<commit_message>
reuniones bitacora, actualizo raiz y modifico datos de prueba Estado y Titular
</commit_message>
<xml_diff>
--- a/Excel/Carga DB Postgres/Estado - CARGADO.xlsx
+++ b/Excel/Carga DB Postgres/Estado - CARGADO.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\playa\asd\sugpaDoc\Excel\Carga DB Postgres\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="360" yWindow="330" windowWidth="18675" windowHeight="7710"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>idestado</t>
   </si>
@@ -24,20 +29,74 @@
     <t>estado</t>
   </si>
   <si>
-    <t>Ingreso</t>
-  </si>
-  <si>
-    <t>Egreso</t>
-  </si>
-  <si>
-    <t>Traslado</t>
+    <t>Adjunta Edicto</t>
+  </si>
+  <si>
+    <t>Adjunta Acta de Entrega</t>
+  </si>
+  <si>
+    <t>Adjunta Expediente Electronico</t>
+  </si>
+  <si>
+    <t>Adjunta Nota de Compactacion</t>
+  </si>
+  <si>
+    <t>Adjunta Remitos de Notificacion</t>
+  </si>
+  <si>
+    <t>Adjunta Cedula de Notificacion</t>
+  </si>
+  <si>
+    <t>Adjunta Dispocisiones y Anexos</t>
+  </si>
+  <si>
+    <t>Traslado a Playa Compactacion</t>
+  </si>
+  <si>
+    <t>Egreso Retira Fuera Policial</t>
+  </si>
+  <si>
+    <t>Egreso Retira Apoderado</t>
+  </si>
+  <si>
+    <t>Egreso Retira Titular</t>
+  </si>
+  <si>
+    <t>Ingreso a Playa</t>
+  </si>
+  <si>
+    <t>Egreso Retira Conducto Autorizado</t>
+  </si>
+  <si>
+    <t>Adjunta Informe de dominio</t>
+  </si>
+  <si>
+    <t>Adjunta Pedido de Secuetro Positivo</t>
+  </si>
+  <si>
+    <t>Adjunta Pedido de Secuetro Negativo</t>
+  </si>
+  <si>
+    <t>Compactado</t>
+  </si>
+  <si>
+    <t>Observado</t>
+  </si>
+  <si>
+    <t>Editado</t>
+  </si>
+  <si>
+    <t>Agrega observacion</t>
+  </si>
+  <si>
+    <t>Traslado de Playa</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +133,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -120,7 +187,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -152,9 +219,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -186,6 +254,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -361,16 +430,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="36.140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,28 +450,172 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -408,24 +624,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>